<commit_message>
Adding swagger documentation, swagger open api code generation and added category post and get apis
</commit_message>
<xml_diff>
--- a/docs/schema_sheet.xlsx
+++ b/docs/schema_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munawarali/Desktop/Repos/Personal/labfarward-programming-test/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{557CC38D-0284-AF4F-87C8-F860BF82F809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E02923-8D2E-4D41-AF1A-593D72DD2DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{CB10507F-6A1C-9843-B19C-17683C8183EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Category</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
+  <si>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
   </si>
 </sst>
 </file>
@@ -137,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -145,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,14 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0249D05E-D1D4-D646-9A79-A65098F364D7}">
-  <dimension ref="D4:I15"/>
+  <dimension ref="D4:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
@@ -504,23 +521,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>5</v>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="4:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="E12" s="3" t="s">
-        <v>6</v>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E13" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="I13" s="5" t="s">
         <v>1</v>
       </c>
@@ -533,6 +577,40 @@
     <row r="15" spans="4:9" x14ac:dyDescent="0.2">
       <c r="I15" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="I16" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Creating categories with attribute definitions rest api
</commit_message>
<xml_diff>
--- a/docs/schema_sheet.xlsx
+++ b/docs/schema_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munawarali/Desktop/Repos/Personal/labfarward-programming-test/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E02923-8D2E-4D41-AF1A-593D72DD2DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDAA0E1-A72D-C84A-8A10-E257C108A593}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{CB10507F-6A1C-9843-B19C-17683C8183EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Category</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Attribute_Definition</t>
   </si>
   <si>
-    <t>Category_Attribute_Definition</t>
-  </si>
-  <si>
     <t>category_id</t>
   </si>
   <si>
@@ -76,6 +73,18 @@
   </si>
   <si>
     <t>updated_at</t>
+  </si>
+  <si>
+    <t>Item_Attribute_Value</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -99,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,8 +133,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -148,6 +163,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -156,11 +182,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,6 +202,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2387600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE197D3-B1EF-2645-83DA-F7E659999E4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6324600" y="2654300"/>
+          <a:ext cx="3289300" cy="1231900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2374900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338C87FD-DAD4-5947-A6B5-15F6C97CC661}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6781800" y="965200"/>
+          <a:ext cx="863600" cy="3124200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49429EF3-D9C1-EF4B-B7BF-AF43709E3444}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2540000" y="977900"/>
+          <a:ext cx="5105400" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,145 +665,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0249D05E-D1D4-D646-9A79-A65098F364D7}">
-  <dimension ref="D4:I20"/>
+  <dimension ref="B4:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
+    <row r="4" spans="2:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="4" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D8" s="7" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="7" t="s">
+    <row r="12" spans="2:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="7" t="s">
+      <c r="I12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="7" t="s">
+      <c r="I13" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="I13" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
       <c r="I14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="I16" s="7" t="s">
-        <v>9</v>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I16" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="5:9" ht="19" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="19" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="7" t="s">
-        <v>13</v>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E24" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>